<commit_message>
Correzione errori di battitura
</commit_message>
<xml_diff>
--- a/requisiti/data dictionary/data dictionary comune.xlsx
+++ b/requisiti/data dictionary/data dictionary comune.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">134 bit</t>
   </si>
   <si>
-    <t xml:space="preserve">Stazione stadale, cellula stradale</t>
+    <t xml:space="preserve">Stazione stradale, cellula stradale</t>
   </si>
   <si>
     <t xml:space="preserve">-36.82065, 175.07823 | “accesa”, -24.82065, 95.07823 | “spenta”</t>
@@ -287,7 +287,7 @@
     <t xml:space="preserve">Notifica</t>
   </si>
   <si>
-    <t xml:space="preserve">Segnalazione dell’avvenimento di un dato evento stradale riguardante il traffico. Può essere indirizzata da un sottosistema verso il sistema centrale o dal sistema centrale verso le applicazioni mobili, oppure anche da quest’ultime verso l’utente.</t>
+    <t xml:space="preserve">Segnalazione dell’avvenimento di un dato evento stradale riguardante il traffico. Può essere indirizzata da un sottosistema verso il sistema centrale o dal sistema centrale verso le applicazioni mobili, oppure anche da queste ultime verso l’utente.</t>
   </si>
   <si>
     <t xml:space="preserve">È un messaggio che indica il tipo di evento e la posizione dell’evento.</t>
@@ -371,13 +371,13 @@
     <t xml:space="preserve">Posizione </t>
   </si>
   <si>
-    <t xml:space="preserve">Notifica, dati di traffco, mappa, conteggio, posizione,</t>
+    <t xml:space="preserve">Notifica, dati di traffico, mappa, conteggio, posizione,</t>
   </si>
   <si>
     <t xml:space="preserve">Veicolo</t>
   </si>
   <si>
-    <t xml:space="preserve">Automobile su cui è installata una centralina auto (oppure unità contata dalla centralina stradale oppure mezzo di trasporto dell’utente che comunica con l’app moble)</t>
+    <t xml:space="preserve">Automobile su cui è installata una centralina auto (oppure unità contata dalla centralina stradale oppure mezzo di trasporto dell’utente che comunica con l’app mobile)</t>
   </si>
   <si>
     <t xml:space="preserve">Dato identificativo di una specifica auto con la relativa posizione e velocità</t>
@@ -528,7 +528,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,10 +542,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -636,25 +632,25 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="55.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="56.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="55.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="27.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="37.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="8.67"/>
   </cols>
   <sheetData>
@@ -703,7 +699,7 @@
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -712,8 +708,8 @@
       <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
@@ -772,8 +768,8 @@
       <c r="F4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="4" t="s">
         <v>34</v>
       </c>
@@ -925,10 +921,10 @@
       <c r="F9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="4" t="s">
         <v>78</v>
       </c>
@@ -984,7 +980,7 @@
       <c r="G11" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="4" t="s">
         <v>93</v>
       </c>
@@ -1064,12 +1060,12 @@
       <c r="D14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="4" t="s">
         <v>114</v>
       </c>

</xml_diff>